<commit_message>
Zmieniono dane w tabeli
</commit_message>
<xml_diff>
--- a/DATA/1.Wypadki_ogolem_smiertleni_ranni_WOJ.xlsx
+++ b/DATA/1.Wypadki_ogolem_smiertleni_ranni_WOJ.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24806"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_9248486D44C93C52631DEA188F3E8C1851038387" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE4CE1D9-059E-4E88-8FDA-84DE8FBD2668}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="11_9248486D44C93C52631DEA188F3E8C1851038387" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6216B91A-0DDC-4972-9008-605121E11C2E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -178,9 +178,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -719,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,7 +760,7 @@
         <v>3202</v>
       </c>
       <c r="E2" s="6">
-        <v>3202</v>
+        <v>42545</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -780,7 +777,7 @@
         <v>242</v>
       </c>
       <c r="E3" s="6">
-        <v>242</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -797,7 +794,7 @@
         <v>179</v>
       </c>
       <c r="E4" s="6">
-        <v>179</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -814,7 +811,7 @@
         <v>195</v>
       </c>
       <c r="E5" s="6">
-        <v>195</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -831,7 +828,7 @@
         <v>81</v>
       </c>
       <c r="E6" s="6">
-        <v>81</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -848,7 +845,7 @@
         <v>256</v>
       </c>
       <c r="E7" s="6">
-        <v>256</v>
+        <v>4807</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -865,7 +862,7 @@
         <v>234</v>
       </c>
       <c r="E8" s="6">
-        <v>234</v>
+        <v>4805</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -882,7 +879,7 @@
         <v>518</v>
       </c>
       <c r="E9" s="6">
-        <v>518</v>
+        <v>5211</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -899,7 +896,7 @@
         <v>104</v>
       </c>
       <c r="E10" s="6">
-        <v>104</v>
+        <v>857</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -916,7 +913,7 @@
         <v>144</v>
       </c>
       <c r="E11" s="6">
-        <v>144</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -933,7 +930,7 @@
         <v>126</v>
       </c>
       <c r="E12" s="6">
-        <v>126</v>
+        <v>793</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -950,7 +947,7 @@
         <v>181</v>
       </c>
       <c r="E13" s="6">
-        <v>181</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -967,7 +964,7 @@
         <v>249</v>
       </c>
       <c r="E14" s="6">
-        <v>249</v>
+        <v>5324</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -984,7 +981,7 @@
         <v>130</v>
       </c>
       <c r="E15" s="6">
-        <v>130</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1001,7 +998,7 @@
         <v>148</v>
       </c>
       <c r="E16" s="6">
-        <v>148</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1018,7 +1015,7 @@
         <v>268</v>
       </c>
       <c r="E17" s="6">
-        <v>268</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1035,7 +1032,7 @@
         <v>147</v>
       </c>
       <c r="E18" s="6">
-        <v>147</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1341,7 +1338,7 @@
         <v>3026</v>
       </c>
       <c r="E36" s="6">
-        <v>3026</v>
+        <v>40766</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1358,7 +1355,7 @@
         <v>226</v>
       </c>
       <c r="E37" s="6">
-        <v>226</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1375,7 +1372,7 @@
         <v>178</v>
       </c>
       <c r="E38" s="6">
-        <v>178</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1392,7 +1389,7 @@
         <v>178</v>
       </c>
       <c r="E39" s="6">
-        <v>178</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1409,7 +1406,7 @@
         <v>113</v>
       </c>
       <c r="E40" s="6">
-        <v>113</v>
+        <v>878</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1426,7 +1423,7 @@
         <v>214</v>
       </c>
       <c r="E41" s="6">
-        <v>214</v>
+        <v>5298</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1443,7 +1440,7 @@
         <v>185</v>
       </c>
       <c r="E42" s="6">
-        <v>185</v>
+        <v>4764</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1460,7 +1457,7 @@
         <v>508</v>
       </c>
       <c r="E43" s="6">
-        <v>508</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1477,7 +1474,7 @@
         <v>99</v>
       </c>
       <c r="E44" s="6">
-        <v>99</v>
+        <v>859</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1494,7 +1491,7 @@
         <v>141</v>
       </c>
       <c r="E45" s="6">
-        <v>141</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1511,7 +1508,7 @@
         <v>120</v>
       </c>
       <c r="E46" s="6">
-        <v>120</v>
+        <v>834</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1528,7 +1525,7 @@
         <v>144</v>
       </c>
       <c r="E47" s="6">
-        <v>144</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1545,7 +1542,7 @@
         <v>257</v>
       </c>
       <c r="E48" s="6">
-        <v>257</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1562,7 +1559,7 @@
         <v>107</v>
       </c>
       <c r="E49" s="6">
-        <v>107</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1579,7 +1576,7 @@
         <v>158</v>
       </c>
       <c r="E50" s="6">
-        <v>158</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1596,7 +1593,7 @@
         <v>249</v>
       </c>
       <c r="E51" s="6">
-        <v>249</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1613,7 +1610,7 @@
         <v>149</v>
       </c>
       <c r="E52" s="6">
-        <v>149</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1627,10 +1624,10 @@
         <v>32760</v>
       </c>
       <c r="D53" s="6">
-        <v>32760</v>
+        <v>2831</v>
       </c>
       <c r="E53" s="6">
-        <v>32760</v>
+        <v>39466</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1644,10 +1641,10 @@
         <v>2183</v>
       </c>
       <c r="D54" s="6">
-        <v>2183</v>
+        <v>219</v>
       </c>
       <c r="E54" s="6">
-        <v>2183</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1661,10 +1658,10 @@
         <v>949</v>
       </c>
       <c r="D55" s="6">
-        <v>949</v>
+        <v>151</v>
       </c>
       <c r="E55" s="6">
-        <v>949</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1678,10 +1675,10 @@
         <v>1242</v>
       </c>
       <c r="D56" s="6">
-        <v>1242</v>
+        <v>157</v>
       </c>
       <c r="E56" s="6">
-        <v>1242</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1695,10 +1692,10 @@
         <v>682</v>
       </c>
       <c r="D57" s="6">
-        <v>682</v>
+        <v>84</v>
       </c>
       <c r="E57" s="6">
-        <v>682</v>
+        <v>855</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1712,10 +1709,10 @@
         <v>3787</v>
       </c>
       <c r="D58" s="6">
-        <v>3787</v>
+        <v>219</v>
       </c>
       <c r="E58" s="6">
-        <v>3787</v>
+        <v>4750</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1729,10 +1726,10 @@
         <v>3612</v>
       </c>
       <c r="D59" s="6">
-        <v>3612</v>
+        <v>194</v>
       </c>
       <c r="E59" s="6">
-        <v>3612</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1746,10 +1743,10 @@
         <v>4048</v>
       </c>
       <c r="D60" s="6">
-        <v>4048</v>
+        <v>464</v>
       </c>
       <c r="E60" s="6">
-        <v>4048</v>
+        <v>4754</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1763,10 +1760,10 @@
         <v>700</v>
       </c>
       <c r="D61" s="6">
-        <v>700</v>
+        <v>78</v>
       </c>
       <c r="E61" s="6">
-        <v>700</v>
+        <v>849</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1780,10 +1777,10 @@
         <v>1710</v>
       </c>
       <c r="D62" s="6">
-        <v>1710</v>
+        <v>124</v>
       </c>
       <c r="E62" s="6">
-        <v>1710</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1797,10 +1794,10 @@
         <v>693</v>
       </c>
       <c r="D63" s="6">
-        <v>693</v>
+        <v>114</v>
       </c>
       <c r="E63" s="6">
-        <v>693</v>
+        <v>802</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1814,10 +1811,10 @@
         <v>2608</v>
       </c>
       <c r="D64" s="6">
-        <v>2608</v>
+        <v>134</v>
       </c>
       <c r="E64" s="6">
-        <v>2608</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1831,10 +1828,10 @@
         <v>3502</v>
       </c>
       <c r="D65" s="6">
-        <v>3502</v>
+        <v>246</v>
       </c>
       <c r="E65" s="6">
-        <v>3502</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1848,10 +1845,10 @@
         <v>1235</v>
       </c>
       <c r="D66" s="6">
-        <v>1235</v>
+        <v>115</v>
       </c>
       <c r="E66" s="6">
-        <v>1235</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1865,10 +1862,10 @@
         <v>1455</v>
       </c>
       <c r="D67" s="6">
-        <v>1455</v>
+        <v>118</v>
       </c>
       <c r="E67" s="6">
-        <v>1455</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1882,10 +1879,10 @@
         <v>3122</v>
       </c>
       <c r="D68" s="6">
-        <v>3122</v>
+        <v>294</v>
       </c>
       <c r="E68" s="6">
-        <v>3122</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1899,10 +1896,10 @@
         <v>1232</v>
       </c>
       <c r="D69" s="6">
-        <v>1232</v>
+        <v>120</v>
       </c>
       <c r="E69" s="6">
-        <v>1232</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2484,10 +2481,10 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="7" t="s">
+      <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B104" s="9">
+      <c r="B104" s="1">
         <v>2020</v>
       </c>
       <c r="C104" s="6">
@@ -2501,10 +2498,10 @@
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B105" s="9">
+      <c r="B105" s="1">
         <v>2020</v>
       </c>
       <c r="C105" s="6">
@@ -2518,10 +2515,10 @@
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B106" s="9">
+      <c r="B106" s="1">
         <v>2020</v>
       </c>
       <c r="C106" s="6">
@@ -2535,10 +2532,10 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="9">
+      <c r="B107" s="1">
         <v>2020</v>
       </c>
       <c r="C107" s="6">
@@ -2552,10 +2549,10 @@
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B108" s="9">
+      <c r="B108" s="1">
         <v>2020</v>
       </c>
       <c r="C108" s="6">
@@ -2569,10 +2566,10 @@
       </c>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B109" s="9">
+      <c r="B109" s="1">
         <v>2020</v>
       </c>
       <c r="C109" s="6">
@@ -2586,10 +2583,10 @@
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B110" s="9">
+      <c r="B110" s="1">
         <v>2020</v>
       </c>
       <c r="C110" s="6">
@@ -2603,10 +2600,10 @@
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="8" t="s">
+      <c r="A111" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="9">
+      <c r="B111" s="1">
         <v>2020</v>
       </c>
       <c r="C111" s="6">
@@ -2620,10 +2617,10 @@
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B112" s="9">
+      <c r="B112" s="1">
         <v>2020</v>
       </c>
       <c r="C112" s="6">
@@ -2637,10 +2634,10 @@
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B113" s="9">
+      <c r="B113" s="1">
         <v>2020</v>
       </c>
       <c r="C113" s="6">
@@ -2654,10 +2651,10 @@
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B114" s="9">
+      <c r="B114" s="1">
         <v>2020</v>
       </c>
       <c r="C114" s="6">
@@ -2671,10 +2668,10 @@
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="8" t="s">
+      <c r="A115" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B115" s="9">
+      <c r="B115" s="1">
         <v>2020</v>
       </c>
       <c r="C115" s="6">
@@ -2688,10 +2685,10 @@
       </c>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B116" s="9">
+      <c r="B116" s="1">
         <v>2020</v>
       </c>
       <c r="C116" s="6">
@@ -2705,10 +2702,10 @@
       </c>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="8" t="s">
+      <c r="A117" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B117" s="9">
+      <c r="B117" s="1">
         <v>2020</v>
       </c>
       <c r="C117" s="6">
@@ -2722,10 +2719,10 @@
       </c>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B118" s="9">
+      <c r="B118" s="1">
         <v>2020</v>
       </c>
       <c r="C118" s="6">
@@ -2739,10 +2736,10 @@
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B119" s="9">
+      <c r="B119" s="1">
         <v>2020</v>
       </c>
       <c r="C119" s="6">
@@ -2756,10 +2753,10 @@
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B120" s="9">
+      <c r="B120" s="1">
         <v>2020</v>
       </c>
       <c r="C120" s="6">

</xml_diff>